<commit_message>
add email already exists check; append test name in reports; overload click method with element name for reports;
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/regression.xlsx
+++ b/src/test/resources/excel/regression.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>testName</t>
   </si>
@@ -34,6 +34,9 @@
     <t>password</t>
   </si>
   <si>
+    <t>confirmPassword</t>
+  </si>
+  <si>
     <t>RegisterUser_ValidRequest</t>
   </si>
   <si>
@@ -53,6 +56,18 @@
   </si>
   <si>
     <t>RANDOM_PASSWORD</t>
+  </si>
+  <si>
+    <t>RegisterUser_EmailAlreadyRegistered</t>
+  </si>
+  <si>
+    <t>Warning: E-Mail Address is already registered!</t>
+  </si>
+  <si>
+    <t>abcd@gmail.com</t>
+  </si>
+  <si>
+    <t>1234567891</t>
   </si>
 </sst>
 </file>
@@ -327,13 +342,14 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.75"/>
-    <col customWidth="1" min="2" max="2" width="15.88"/>
+    <col customWidth="1" min="1" max="1" width="30.0"/>
+    <col customWidth="1" min="2" max="2" width="35.88"/>
     <col customWidth="1" min="3" max="3" width="17.0"/>
     <col customWidth="1" min="4" max="4" width="16.63"/>
     <col customWidth="1" min="5" max="5" width="15.63"/>
     <col customWidth="1" min="6" max="6" width="17.5"/>
     <col customWidth="1" min="7" max="7" width="19.13"/>
+    <col customWidth="1" min="8" max="8" width="19.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -358,28 +374,60 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>